<commit_message>
POL-3063: using internal sanitizer (#2469)
* POL-3063: using internal sanitizer

* POL-3063: missed file

* POL-3063: coverage on sanitizer

* POL-3063: last line of coverage and a rubocop mistake
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_saco_pricings.xlsx
+++ b/spec/fixtures/files/excel/example_saco_pricings.xlsx
@@ -6,17 +6,17 @@
     <sheet state="visible" name="Africa" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_D229C9D2_6D8E_434C_9096_57E27DF2AD07_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_6CC3DFFF_7019_40CA_8175_39D008380C8A_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_7166CA3A_83F5_4C08_9D7F_26B8ADF02A24_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_7CE7BA65_B089_4AA6_935C_A998B0653E7D_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_68DFCC14_0523_47BB_B77A_F517A28BB91C_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D8983E15_4FC1_4A80_93C5_4000FD62EAFE_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FB3C7818_4343_4A28_8E26_044A3EA3FFB6_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_65C347E1_C998_4DAB_AADA_CAA2A50B84A3_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7166CA3A-83F5-4C08-9D7F-26B8ADF02A24}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7CE7BA65-B089-4AA6-935C-A998B0653E7D}" name="mbc - Persönliche Ansicht"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6CC3DFFF-7019-40CA-8175-39D008380C8A}" name="Filter 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D229C9D2-6D8E-434C-9096-57E27DF2AD07}" name="jst - Persönliche Ansicht"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{65C347E1-C998-4DAB-AADA-CAA2A50B84A3}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB3C7818-4343-4A28-8E26-044A3EA3FFB6}" name="mbc - Persönliche Ansicht"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8983E15-4FC1-4A80-93C5-4000FD62EAFE}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{68DFCC14-0523-47BB-B77A-F517A28BB91C}" name="jst - Persönliche Ansicht"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="84">
   <si>
     <t>INTERNAL</t>
   </si>
@@ -564,7 +564,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -600,6 +600,9 @@
     <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -629,9 +632,6 @@
     </xf>
     <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -1567,7 +1567,9 @@
       <c r="BN3" s="25"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="27"/>
+      <c r="A4" s="27" t="s">
+        <v>74</v>
+      </c>
       <c r="B4" s="28" t="s">
         <v>63</v>
       </c>
@@ -1636,7 +1638,7 @@
       <c r="Y4" s="39">
         <v>240.0</v>
       </c>
-      <c r="Z4" s="27" t="s">
+      <c r="Z4" s="40" t="s">
         <v>71</v>
       </c>
       <c r="AA4" s="38" t="s">
@@ -1666,92 +1668,92 @@
       <c r="AI4" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="AJ4" s="40">
+      <c r="AJ4" s="41">
         <v>30.0</v>
       </c>
-      <c r="AK4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM4" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN4" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO4" s="43">
+      <c r="AK4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO4" s="44">
         <v>75.0</v>
       </c>
-      <c r="AP4" s="44">
+      <c r="AP4" s="45">
         <v>75.0</v>
       </c>
-      <c r="AQ4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ4" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA4" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BC4" s="41" t="s">
+      <c r="AQ4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ4" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA4" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC4" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="BD4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BF4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BG4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BH4" s="46">
+      <c r="BD4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH4" s="47">
         <v>15.0</v>
       </c>
-      <c r="BI4" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="BJ4" s="41"/>
-      <c r="BK4" s="47"/>
-      <c r="BL4" s="48"/>
-      <c r="BM4" s="49"/>
-      <c r="BN4" s="48"/>
+      <c r="BI4" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ4" s="42"/>
+      <c r="BK4" s="48"/>
+      <c r="BL4" s="49"/>
+      <c r="BM4" s="50"/>
+      <c r="BN4" s="49"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -1822,7 +1824,7 @@
       <c r="Y5" s="39">
         <v>240.0</v>
       </c>
-      <c r="Z5" s="27" t="s">
+      <c r="Z5" s="40" t="s">
         <v>71</v>
       </c>
       <c r="AA5" s="38" t="s">
@@ -1852,92 +1854,92 @@
       <c r="AI5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="AJ5" s="40">
+      <c r="AJ5" s="41">
         <v>30.0</v>
       </c>
-      <c r="AK5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM5" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN5" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO5" s="42">
+      <c r="AK5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM5" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN5" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO5" s="43">
         <v>75.0</v>
       </c>
       <c r="AP5" s="53">
         <v>75.0</v>
       </c>
-      <c r="AQ5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ5" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA5" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BC5" s="41" t="s">
+      <c r="AQ5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ5" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA5" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="BD5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BF5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BG5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BH5" s="46">
+      <c r="BD5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH5" s="47">
         <v>15.0</v>
       </c>
-      <c r="BI5" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="47"/>
+      <c r="BI5" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ5" s="42"/>
+      <c r="BK5" s="48"/>
       <c r="BL5" s="54"/>
-      <c r="BM5" s="49"/>
-      <c r="BN5" s="48"/>
+      <c r="BM5" s="50"/>
+      <c r="BN5" s="49"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="27"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="28" t="s">
         <v>63</v>
       </c>
@@ -2006,7 +2008,7 @@
       <c r="Y6" s="39">
         <v>200.0</v>
       </c>
-      <c r="Z6" s="27" t="s">
+      <c r="Z6" s="40" t="s">
         <v>71</v>
       </c>
       <c r="AA6" s="38" t="s">
@@ -2036,92 +2038,92 @@
       <c r="AI6" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="AJ6" s="40">
+      <c r="AJ6" s="41">
         <v>30.0</v>
       </c>
-      <c r="AK6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM6" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN6" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO6" s="42">
+      <c r="AK6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM6" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN6" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO6" s="43">
         <v>75.0</v>
       </c>
       <c r="AP6" s="53">
         <v>75.0</v>
       </c>
-      <c r="AQ6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ6" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA6" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BC6" s="41" t="s">
+      <c r="AQ6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ6" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA6" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC6" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="BD6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BF6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BG6" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="BH6" s="46">
+      <c r="BD6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG6" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH6" s="47">
         <v>15.0</v>
       </c>
-      <c r="BI6" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="BJ6" s="41"/>
-      <c r="BK6" s="47"/>
+      <c r="BI6" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ6" s="42"/>
+      <c r="BK6" s="48"/>
       <c r="BL6" s="54"/>
-      <c r="BM6" s="49"/>
-      <c r="BN6" s="48"/>
+      <c r="BM6" s="50"/>
+      <c r="BN6" s="49"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="27"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="28" t="s">
         <v>63</v>
       </c>
@@ -2190,7 +2192,7 @@
       <c r="Y7" s="39">
         <v>200.0</v>
       </c>
-      <c r="Z7" s="27" t="s">
+      <c r="Z7" s="40" t="s">
         <v>71</v>
       </c>
       <c r="AA7" s="38" t="s">
@@ -2220,19 +2222,19 @@
       <c r="AI7" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="AJ7" s="40">
+      <c r="AJ7" s="41">
         <v>30.0</v>
       </c>
-      <c r="AK7" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL7" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM7" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN7" s="42" t="s">
+      <c r="AK7" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL7" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM7" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN7" s="43" t="s">
         <v>70</v>
       </c>
       <c r="AO7" s="57">
@@ -2253,10 +2255,10 @@
       <c r="AT7" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="AU7" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV7" s="41" t="s">
+      <c r="AU7" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV7" s="42" t="s">
         <v>73</v>
       </c>
       <c r="AW7" s="59" t="s">
@@ -2268,10 +2270,10 @@
       <c r="AY7" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="AZ7" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA7" s="45" t="s">
+      <c r="AZ7" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA7" s="46" t="s">
         <v>70</v>
       </c>
       <c r="BB7" s="58" t="s">
@@ -2292,17 +2294,17 @@
       <c r="BG7" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="BH7" s="46">
+      <c r="BH7" s="47">
         <v>15.0</v>
       </c>
       <c r="BI7" s="60" t="s">
         <v>73</v>
       </c>
       <c r="BJ7" s="58"/>
-      <c r="BK7" s="47"/>
-      <c r="BL7" s="48"/>
-      <c r="BM7" s="49"/>
-      <c r="BN7" s="48"/>
+      <c r="BK7" s="48"/>
+      <c r="BL7" s="49"/>
+      <c r="BM7" s="50"/>
+      <c r="BN7" s="49"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="61"/>
@@ -4269,7 +4271,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7CE7BA65-B089-4AA6-935C-A998B0653E7D}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FB3C7818-4343-4A28-8E26-044A3EA3FFB6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
@@ -4277,7 +4279,7 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{6CC3DFFF-7019-40CA-8175-39D008380C8A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D8983E15-4FC1-4A80-93C5-4000FD62EAFE}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
@@ -4285,7 +4287,7 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{D229C9D2-6D8E-434C-9096-57E27DF2AD07}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{68DFCC14-0523-47BB-B77A-F517A28BB91C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
@@ -4293,7 +4295,7 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{7166CA3A-83F5-4C08-9D7F-26B8ADF02A24}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{65C347E1-C998-4DAB-AADA-CAA2A50B84A3}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
POL-3157: Reject N/A pricings entirely from SACO uploader (#2540)
* POL-3157: init

* POL3157: remedied

* POL-3157: resolved and specced

* POL-3157: using explicit value rather than nil to find rows

* POL-3157: placeholder one word

* POL-3157: fixed specs

Co-authored-by: Ajith Kumar <88225952+ajithatimc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_saco_pricings.xlsx
+++ b/spec/fixtures/files/excel/example_saco_pricings.xlsx
@@ -6,17 +6,17 @@
     <sheet state="visible" name="Africa" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_68DFCC14_0523_47BB_B77A_F517A28BB91C_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D8983E15_4FC1_4A80_93C5_4000FD62EAFE_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_FB3C7818_4343_4A28_8E26_044A3EA3FFB6_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_65C347E1_C998_4DAB_AADA_CAA2A50B84A3_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B7FEAD40_3014_4592_862A_43375AC0CF55_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_15618BF6_7F2C_45DE_8AC8_B0FB1C498E50_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_CD1ADC1F_EDD1_4928_9B54_5CE003589629_.wvu.FilterData">Africa!$A$1:$BK$10</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_483C286D_37C2_478D_A8B5_55DAECA2C6C9_.wvu.FilterData">Africa!$A$1:$BK$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{65C347E1-C998-4DAB-AADA-CAA2A50B84A3}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB3C7818-4343-4A28-8E26-044A3EA3FFB6}" name="mbc - Persönliche Ansicht"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8983E15-4FC1-4A80-93C5-4000FD62EAFE}" name="Filter 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{68DFCC14-0523-47BB-B77A-F517A28BB91C}" name="jst - Persönliche Ansicht"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B7FEAD40-3014-4592-862A-43375AC0CF55}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{CD1ADC1F-EDD1-4928-9B54-5CE003589629}" name="mbc - Persönliche Ansicht"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{15618BF6-7F2C-45DE-8AC8-B0FB1C498E50}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{483C286D-37C2-478D-A8B5-55DAECA2C6C9}" name="jst - Persönliche Ansicht"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="85">
   <si>
     <t>INTERNAL</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>AOLAD</t>
+  </si>
+  <si>
+    <t>SSC</t>
   </si>
 </sst>
 </file>
@@ -292,14 +295,20 @@
     <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
     <numFmt numFmtId="168" formatCode="#,##0.00 [$EUR]"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -481,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -512,151 +521,151 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="10" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="11" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="5" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="5" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -665,71 +674,77 @@
     <xf borderId="14" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="12" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -951,53 +966,53 @@
       <selection activeCell="E2" sqref="E2" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.57"/>
-    <col customWidth="1" min="2" max="2" width="31.43"/>
-    <col customWidth="1" min="3" max="3" width="26.0"/>
-    <col customWidth="1" min="4" max="4" width="22.0"/>
-    <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="6" width="24.57"/>
-    <col customWidth="1" min="7" max="7" width="12.71"/>
-    <col customWidth="1" min="8" max="8" width="20.0"/>
-    <col customWidth="1" min="9" max="9" width="20.57"/>
-    <col customWidth="1" min="10" max="10" width="21.57"/>
-    <col customWidth="1" min="11" max="13" width="10.43"/>
-    <col customWidth="1" min="14" max="14" width="24.57"/>
-    <col customWidth="1" min="15" max="16" width="10.29"/>
-    <col customWidth="1" min="17" max="17" width="22.0"/>
-    <col customWidth="1" min="18" max="19" width="21.29"/>
-    <col customWidth="1" min="20" max="20" width="21.57"/>
-    <col customWidth="1" min="21" max="22" width="21.0"/>
-    <col customWidth="1" min="23" max="24" width="14.43"/>
-    <col customWidth="1" min="25" max="25" width="8.86"/>
-    <col customWidth="1" min="26" max="26" width="22.0"/>
-    <col customWidth="1" min="27" max="28" width="21.29"/>
-    <col customWidth="1" min="29" max="29" width="21.57"/>
-    <col customWidth="1" min="30" max="31" width="21.0"/>
-    <col customWidth="1" min="32" max="33" width="13.86"/>
-    <col customWidth="1" min="34" max="35" width="10.57"/>
-    <col customWidth="1" min="36" max="36" width="8.29"/>
-    <col customWidth="1" min="37" max="38" width="15.57"/>
-    <col customWidth="1" min="39" max="40" width="17.14"/>
-    <col customWidth="1" min="41" max="42" width="44.71"/>
-    <col customWidth="1" min="43" max="44" width="33.43"/>
-    <col customWidth="1" min="45" max="46" width="17.43"/>
-    <col customWidth="1" min="47" max="48" width="32.0"/>
-    <col customWidth="1" min="49" max="49" width="32.29"/>
-    <col customWidth="1" min="50" max="50" width="23.14"/>
-    <col customWidth="1" min="51" max="51" width="33.71"/>
-    <col customWidth="1" min="52" max="53" width="23.86"/>
-    <col customWidth="1" min="54" max="54" width="59.0"/>
-    <col customWidth="1" min="55" max="55" width="33.86"/>
-    <col customWidth="1" min="56" max="57" width="16.57"/>
-    <col customWidth="1" min="58" max="59" width="16.14"/>
-    <col customWidth="1" min="60" max="60" width="17.0"/>
-    <col customWidth="1" min="61" max="61" width="13.86"/>
-    <col customWidth="1" min="62" max="62" width="34.57"/>
-    <col customWidth="1" min="63" max="63" width="69.43"/>
-    <col customWidth="1" min="64" max="66" width="11.57"/>
+    <col customWidth="1" min="1" max="1" width="11.88"/>
+    <col customWidth="1" min="2" max="2" width="27.5"/>
+    <col customWidth="1" min="3" max="3" width="22.75"/>
+    <col customWidth="1" min="4" max="4" width="19.25"/>
+    <col customWidth="1" min="5" max="5" width="12.13"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="11.13"/>
+    <col customWidth="1" min="8" max="8" width="17.5"/>
+    <col customWidth="1" min="9" max="9" width="18.0"/>
+    <col customWidth="1" min="10" max="10" width="18.88"/>
+    <col customWidth="1" min="11" max="13" width="9.13"/>
+    <col customWidth="1" min="14" max="14" width="21.5"/>
+    <col customWidth="1" min="15" max="16" width="9.0"/>
+    <col customWidth="1" min="17" max="17" width="19.25"/>
+    <col customWidth="1" min="18" max="19" width="18.63"/>
+    <col customWidth="1" min="20" max="20" width="18.88"/>
+    <col customWidth="1" min="21" max="22" width="18.38"/>
+    <col customWidth="1" min="23" max="24" width="12.63"/>
+    <col customWidth="1" min="25" max="25" width="7.75"/>
+    <col customWidth="1" min="26" max="26" width="19.25"/>
+    <col customWidth="1" min="27" max="28" width="18.63"/>
+    <col customWidth="1" min="29" max="29" width="18.88"/>
+    <col customWidth="1" min="30" max="31" width="18.38"/>
+    <col customWidth="1" min="32" max="33" width="12.13"/>
+    <col customWidth="1" min="34" max="35" width="9.25"/>
+    <col customWidth="1" min="36" max="36" width="7.25"/>
+    <col customWidth="1" min="37" max="38" width="13.63"/>
+    <col customWidth="1" min="39" max="40" width="15.0"/>
+    <col customWidth="1" min="41" max="42" width="39.13"/>
+    <col customWidth="1" min="43" max="44" width="29.25"/>
+    <col customWidth="1" min="45" max="46" width="15.25"/>
+    <col customWidth="1" min="47" max="48" width="28.0"/>
+    <col customWidth="1" min="49" max="49" width="28.25"/>
+    <col customWidth="1" min="50" max="50" width="20.25"/>
+    <col customWidth="1" min="51" max="51" width="29.5"/>
+    <col customWidth="1" min="52" max="53" width="20.88"/>
+    <col customWidth="1" min="54" max="54" width="51.63"/>
+    <col customWidth="1" min="55" max="55" width="29.63"/>
+    <col customWidth="1" min="56" max="57" width="14.5"/>
+    <col customWidth="1" min="58" max="59" width="14.13"/>
+    <col customWidth="1" min="60" max="60" width="14.88"/>
+    <col customWidth="1" min="61" max="61" width="12.13"/>
+    <col customWidth="1" min="62" max="62" width="30.25"/>
+    <col customWidth="1" min="63" max="63" width="60.75"/>
+    <col customWidth="1" min="64" max="66" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
@@ -2679,724 +2694,904 @@
       <c r="BN9" s="79"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="R10" s="84"/>
-      <c r="S10" s="84"/>
-      <c r="W10" s="85"/>
-      <c r="X10" s="85"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="63">
+        <v>44440.0</v>
+      </c>
+      <c r="J10" s="81">
+        <v>44530.0</v>
+      </c>
+      <c r="K10" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="M10" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="P10" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="38">
+        <v>235.0</v>
+      </c>
+      <c r="S10" s="38">
+        <v>470.0</v>
+      </c>
+      <c r="T10" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="U10" s="82">
+        <v>255.0</v>
+      </c>
+      <c r="V10" s="82">
+        <v>520.0</v>
+      </c>
+      <c r="W10" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="X10" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y10" s="71">
+        <v>210.0</v>
+      </c>
+      <c r="Z10" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA10" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB10" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD10" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE10" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF10" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG10" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH10" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI10" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ10" s="74">
+        <v>29.0</v>
+      </c>
+      <c r="AK10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO10" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP10" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ10" s="73">
+        <v>200.0</v>
+      </c>
+      <c r="BA10" s="73">
+        <v>200.0</v>
+      </c>
+      <c r="BB10" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="BC10" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG10" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH10" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI10" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ10" s="75"/>
+      <c r="BK10" s="83"/>
+      <c r="BL10" s="79"/>
+      <c r="BM10" s="79"/>
+      <c r="BN10" s="79"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="R11" s="84"/>
-      <c r="S11" s="84"/>
-      <c r="W11" s="85"/>
-      <c r="X11" s="85"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="R12" s="84"/>
-      <c r="S12" s="84"/>
-      <c r="W12" s="85"/>
-      <c r="X12" s="85"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="R13" s="84"/>
-      <c r="S13" s="84"/>
-      <c r="W13" s="85"/>
-      <c r="X13" s="85"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="R14" s="84"/>
-      <c r="S14" s="84"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="85"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="W14" s="87"/>
+      <c r="X14" s="87"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="R15" s="84"/>
-      <c r="S15" s="84"/>
-      <c r="W15" s="85"/>
-      <c r="X15" s="85"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="W15" s="87"/>
+      <c r="X15" s="87"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="W16" s="85"/>
-      <c r="X16" s="85"/>
+      <c r="R16" s="86"/>
+      <c r="S16" s="86"/>
+      <c r="W16" s="87"/>
+      <c r="X16" s="87"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="R17" s="84"/>
-      <c r="S17" s="84"/>
-      <c r="W17" s="85"/>
-      <c r="X17" s="85"/>
+      <c r="R17" s="86"/>
+      <c r="S17" s="86"/>
+      <c r="W17" s="87"/>
+      <c r="X17" s="87"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="R18" s="84"/>
-      <c r="S18" s="84"/>
-      <c r="W18" s="85"/>
-      <c r="X18" s="85"/>
+      <c r="R18" s="86"/>
+      <c r="S18" s="86"/>
+      <c r="W18" s="87"/>
+      <c r="X18" s="87"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="R19" s="84"/>
-      <c r="S19" s="84"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="85"/>
+      <c r="R19" s="86"/>
+      <c r="S19" s="86"/>
+      <c r="W19" s="87"/>
+      <c r="X19" s="87"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="R20" s="84"/>
-      <c r="S20" s="84"/>
-      <c r="W20" s="85"/>
-      <c r="X20" s="85"/>
+      <c r="R20" s="86"/>
+      <c r="S20" s="86"/>
+      <c r="W20" s="87"/>
+      <c r="X20" s="87"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="R21" s="84"/>
-      <c r="S21" s="84"/>
-      <c r="W21" s="85"/>
-      <c r="X21" s="85"/>
+      <c r="R21" s="86"/>
+      <c r="S21" s="86"/>
+      <c r="W21" s="87"/>
+      <c r="X21" s="87"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
-      <c r="W22" s="85"/>
-      <c r="X22" s="85"/>
+      <c r="R22" s="86"/>
+      <c r="S22" s="86"/>
+      <c r="W22" s="87"/>
+      <c r="X22" s="87"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="R23" s="84"/>
-      <c r="S23" s="84"/>
-      <c r="W23" s="85"/>
-      <c r="X23" s="85"/>
+      <c r="R23" s="86"/>
+      <c r="S23" s="86"/>
+      <c r="W23" s="87"/>
+      <c r="X23" s="87"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="R24" s="84"/>
-      <c r="S24" s="84"/>
-      <c r="W24" s="85"/>
-      <c r="X24" s="85"/>
+      <c r="R24" s="86"/>
+      <c r="S24" s="86"/>
+      <c r="W24" s="87"/>
+      <c r="X24" s="87"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="W25" s="85"/>
-      <c r="X25" s="85"/>
+      <c r="R25" s="86"/>
+      <c r="S25" s="86"/>
+      <c r="W25" s="87"/>
+      <c r="X25" s="87"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="R26" s="84"/>
-      <c r="S26" s="84"/>
-      <c r="W26" s="85"/>
-      <c r="X26" s="85"/>
+      <c r="R26" s="86"/>
+      <c r="S26" s="86"/>
+      <c r="W26" s="87"/>
+      <c r="X26" s="87"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="R27" s="84"/>
-      <c r="S27" s="84"/>
-      <c r="W27" s="85"/>
-      <c r="X27" s="85"/>
+      <c r="R27" s="86"/>
+      <c r="S27" s="86"/>
+      <c r="W27" s="87"/>
+      <c r="X27" s="87"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="R28" s="84"/>
-      <c r="S28" s="84"/>
-      <c r="W28" s="85"/>
-      <c r="X28" s="85"/>
+      <c r="R28" s="86"/>
+      <c r="S28" s="86"/>
+      <c r="W28" s="87"/>
+      <c r="X28" s="87"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="R29" s="84"/>
-      <c r="S29" s="84"/>
-      <c r="W29" s="85"/>
-      <c r="X29" s="85"/>
+      <c r="R29" s="86"/>
+      <c r="S29" s="86"/>
+      <c r="W29" s="87"/>
+      <c r="X29" s="87"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="R30" s="84"/>
-      <c r="S30" s="84"/>
-      <c r="W30" s="85"/>
-      <c r="X30" s="85"/>
+      <c r="R30" s="86"/>
+      <c r="S30" s="86"/>
+      <c r="W30" s="87"/>
+      <c r="X30" s="87"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="R31" s="84"/>
-      <c r="S31" s="84"/>
-      <c r="W31" s="85"/>
-      <c r="X31" s="85"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
+      <c r="W31" s="87"/>
+      <c r="X31" s="87"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="R32" s="84"/>
-      <c r="S32" s="84"/>
-      <c r="W32" s="85"/>
-      <c r="X32" s="85"/>
+      <c r="R32" s="86"/>
+      <c r="S32" s="86"/>
+      <c r="W32" s="87"/>
+      <c r="X32" s="87"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="R33" s="84"/>
-      <c r="S33" s="84"/>
-      <c r="W33" s="85"/>
-      <c r="X33" s="85"/>
+      <c r="R33" s="86"/>
+      <c r="S33" s="86"/>
+      <c r="W33" s="87"/>
+      <c r="X33" s="87"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="R34" s="84"/>
-      <c r="S34" s="84"/>
-      <c r="W34" s="85"/>
-      <c r="X34" s="85"/>
+      <c r="R34" s="86"/>
+      <c r="S34" s="86"/>
+      <c r="W34" s="87"/>
+      <c r="X34" s="87"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="R35" s="84"/>
-      <c r="S35" s="84"/>
-      <c r="W35" s="85"/>
-      <c r="X35" s="85"/>
+      <c r="R35" s="86"/>
+      <c r="S35" s="86"/>
+      <c r="W35" s="87"/>
+      <c r="X35" s="87"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="R36" s="84"/>
-      <c r="S36" s="84"/>
-      <c r="W36" s="85"/>
-      <c r="X36" s="85"/>
+      <c r="R36" s="86"/>
+      <c r="S36" s="86"/>
+      <c r="W36" s="87"/>
+      <c r="X36" s="87"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="R37" s="84"/>
-      <c r="S37" s="84"/>
-      <c r="W37" s="85"/>
-      <c r="X37" s="85"/>
+      <c r="R37" s="86"/>
+      <c r="S37" s="86"/>
+      <c r="W37" s="87"/>
+      <c r="X37" s="87"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="R38" s="84"/>
-      <c r="S38" s="84"/>
-      <c r="W38" s="85"/>
-      <c r="X38" s="85"/>
+      <c r="R38" s="86"/>
+      <c r="S38" s="86"/>
+      <c r="W38" s="87"/>
+      <c r="X38" s="87"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="R39" s="84"/>
-      <c r="S39" s="84"/>
-      <c r="W39" s="85"/>
-      <c r="X39" s="85"/>
+      <c r="R39" s="86"/>
+      <c r="S39" s="86"/>
+      <c r="W39" s="87"/>
+      <c r="X39" s="87"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="R40" s="84"/>
-      <c r="S40" s="84"/>
-      <c r="W40" s="85"/>
-      <c r="X40" s="85"/>
+      <c r="R40" s="86"/>
+      <c r="S40" s="86"/>
+      <c r="W40" s="87"/>
+      <c r="X40" s="87"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="R41" s="84"/>
-      <c r="S41" s="84"/>
-      <c r="W41" s="85"/>
-      <c r="X41" s="85"/>
+      <c r="R41" s="86"/>
+      <c r="S41" s="86"/>
+      <c r="W41" s="87"/>
+      <c r="X41" s="87"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="R42" s="84"/>
-      <c r="S42" s="84"/>
-      <c r="W42" s="85"/>
-      <c r="X42" s="85"/>
+      <c r="R42" s="86"/>
+      <c r="S42" s="86"/>
+      <c r="W42" s="87"/>
+      <c r="X42" s="87"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="R43" s="84"/>
-      <c r="S43" s="84"/>
-      <c r="W43" s="85"/>
-      <c r="X43" s="85"/>
+      <c r="R43" s="86"/>
+      <c r="S43" s="86"/>
+      <c r="W43" s="87"/>
+      <c r="X43" s="87"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="R44" s="84"/>
-      <c r="S44" s="84"/>
-      <c r="W44" s="85"/>
-      <c r="X44" s="85"/>
+      <c r="R44" s="86"/>
+      <c r="S44" s="86"/>
+      <c r="W44" s="87"/>
+      <c r="X44" s="87"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="R45" s="84"/>
-      <c r="S45" s="84"/>
-      <c r="W45" s="85"/>
-      <c r="X45" s="85"/>
+      <c r="R45" s="86"/>
+      <c r="S45" s="86"/>
+      <c r="W45" s="87"/>
+      <c r="X45" s="87"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="R46" s="84"/>
-      <c r="S46" s="84"/>
-      <c r="W46" s="85"/>
-      <c r="X46" s="85"/>
+      <c r="R46" s="86"/>
+      <c r="S46" s="86"/>
+      <c r="W46" s="87"/>
+      <c r="X46" s="87"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="R47" s="84"/>
-      <c r="S47" s="84"/>
-      <c r="W47" s="85"/>
-      <c r="X47" s="85"/>
+      <c r="R47" s="86"/>
+      <c r="S47" s="86"/>
+      <c r="W47" s="87"/>
+      <c r="X47" s="87"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="R48" s="84"/>
-      <c r="S48" s="84"/>
-      <c r="W48" s="85"/>
-      <c r="X48" s="85"/>
+      <c r="R48" s="86"/>
+      <c r="S48" s="86"/>
+      <c r="W48" s="87"/>
+      <c r="X48" s="87"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="R49" s="84"/>
-      <c r="S49" s="84"/>
-      <c r="W49" s="85"/>
-      <c r="X49" s="85"/>
+      <c r="R49" s="86"/>
+      <c r="S49" s="86"/>
+      <c r="W49" s="87"/>
+      <c r="X49" s="87"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="R50" s="84"/>
-      <c r="S50" s="84"/>
-      <c r="W50" s="85"/>
-      <c r="X50" s="85"/>
+      <c r="R50" s="86"/>
+      <c r="S50" s="86"/>
+      <c r="W50" s="87"/>
+      <c r="X50" s="87"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="R51" s="84"/>
-      <c r="S51" s="84"/>
-      <c r="W51" s="85"/>
-      <c r="X51" s="85"/>
+      <c r="R51" s="86"/>
+      <c r="S51" s="86"/>
+      <c r="W51" s="87"/>
+      <c r="X51" s="87"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="R52" s="84"/>
-      <c r="S52" s="84"/>
-      <c r="W52" s="85"/>
-      <c r="X52" s="85"/>
+      <c r="R52" s="86"/>
+      <c r="S52" s="86"/>
+      <c r="W52" s="87"/>
+      <c r="X52" s="87"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="R53" s="84"/>
-      <c r="S53" s="84"/>
-      <c r="W53" s="85"/>
-      <c r="X53" s="85"/>
+      <c r="R53" s="86"/>
+      <c r="S53" s="86"/>
+      <c r="W53" s="87"/>
+      <c r="X53" s="87"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="R54" s="84"/>
-      <c r="S54" s="84"/>
-      <c r="W54" s="85"/>
-      <c r="X54" s="85"/>
+      <c r="R54" s="86"/>
+      <c r="S54" s="86"/>
+      <c r="W54" s="87"/>
+      <c r="X54" s="87"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="R55" s="84"/>
-      <c r="S55" s="84"/>
-      <c r="W55" s="85"/>
-      <c r="X55" s="85"/>
+      <c r="R55" s="86"/>
+      <c r="S55" s="86"/>
+      <c r="W55" s="87"/>
+      <c r="X55" s="87"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="R56" s="84"/>
-      <c r="S56" s="84"/>
-      <c r="W56" s="85"/>
-      <c r="X56" s="85"/>
+      <c r="R56" s="86"/>
+      <c r="S56" s="86"/>
+      <c r="W56" s="87"/>
+      <c r="X56" s="87"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="R57" s="84"/>
-      <c r="S57" s="84"/>
-      <c r="W57" s="85"/>
-      <c r="X57" s="85"/>
+      <c r="R57" s="86"/>
+      <c r="S57" s="86"/>
+      <c r="W57" s="87"/>
+      <c r="X57" s="87"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="R58" s="84"/>
-      <c r="S58" s="84"/>
-      <c r="W58" s="85"/>
-      <c r="X58" s="85"/>
+      <c r="R58" s="86"/>
+      <c r="S58" s="86"/>
+      <c r="W58" s="87"/>
+      <c r="X58" s="87"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="R59" s="84"/>
-      <c r="S59" s="84"/>
-      <c r="W59" s="85"/>
-      <c r="X59" s="85"/>
+      <c r="R59" s="86"/>
+      <c r="S59" s="86"/>
+      <c r="W59" s="87"/>
+      <c r="X59" s="87"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="R60" s="84"/>
-      <c r="S60" s="84"/>
-      <c r="W60" s="85"/>
-      <c r="X60" s="85"/>
+      <c r="R60" s="86"/>
+      <c r="S60" s="86"/>
+      <c r="W60" s="87"/>
+      <c r="X60" s="87"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="R61" s="84"/>
-      <c r="S61" s="84"/>
-      <c r="W61" s="85"/>
-      <c r="X61" s="85"/>
+      <c r="R61" s="86"/>
+      <c r="S61" s="86"/>
+      <c r="W61" s="87"/>
+      <c r="X61" s="87"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="R62" s="84"/>
-      <c r="S62" s="84"/>
-      <c r="W62" s="85"/>
-      <c r="X62" s="85"/>
+      <c r="R62" s="86"/>
+      <c r="S62" s="86"/>
+      <c r="W62" s="87"/>
+      <c r="X62" s="87"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="R63" s="84"/>
-      <c r="S63" s="84"/>
-      <c r="W63" s="85"/>
-      <c r="X63" s="85"/>
+      <c r="R63" s="86"/>
+      <c r="S63" s="86"/>
+      <c r="W63" s="87"/>
+      <c r="X63" s="87"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="R64" s="84"/>
-      <c r="S64" s="84"/>
-      <c r="W64" s="85"/>
-      <c r="X64" s="85"/>
+      <c r="R64" s="86"/>
+      <c r="S64" s="86"/>
+      <c r="W64" s="87"/>
+      <c r="X64" s="87"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="R65" s="84"/>
-      <c r="S65" s="84"/>
-      <c r="W65" s="85"/>
-      <c r="X65" s="85"/>
+      <c r="R65" s="86"/>
+      <c r="S65" s="86"/>
+      <c r="W65" s="87"/>
+      <c r="X65" s="87"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="R66" s="84"/>
-      <c r="S66" s="84"/>
-      <c r="W66" s="85"/>
-      <c r="X66" s="85"/>
+      <c r="R66" s="86"/>
+      <c r="S66" s="86"/>
+      <c r="W66" s="87"/>
+      <c r="X66" s="87"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="R67" s="84"/>
-      <c r="S67" s="84"/>
-      <c r="W67" s="85"/>
-      <c r="X67" s="85"/>
+      <c r="R67" s="86"/>
+      <c r="S67" s="86"/>
+      <c r="W67" s="87"/>
+      <c r="X67" s="87"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="R68" s="84"/>
-      <c r="S68" s="84"/>
-      <c r="W68" s="85"/>
-      <c r="X68" s="85"/>
+      <c r="R68" s="86"/>
+      <c r="S68" s="86"/>
+      <c r="W68" s="87"/>
+      <c r="X68" s="87"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="R69" s="84"/>
-      <c r="S69" s="84"/>
-      <c r="W69" s="85"/>
-      <c r="X69" s="85"/>
+      <c r="R69" s="86"/>
+      <c r="S69" s="86"/>
+      <c r="W69" s="87"/>
+      <c r="X69" s="87"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="R70" s="84"/>
-      <c r="S70" s="84"/>
-      <c r="W70" s="85"/>
-      <c r="X70" s="85"/>
+      <c r="R70" s="86"/>
+      <c r="S70" s="86"/>
+      <c r="W70" s="87"/>
+      <c r="X70" s="87"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="R71" s="84"/>
-      <c r="S71" s="84"/>
-      <c r="W71" s="85"/>
-      <c r="X71" s="85"/>
+      <c r="R71" s="86"/>
+      <c r="S71" s="86"/>
+      <c r="W71" s="87"/>
+      <c r="X71" s="87"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="R72" s="84"/>
-      <c r="S72" s="84"/>
-      <c r="W72" s="85"/>
-      <c r="X72" s="85"/>
+      <c r="R72" s="86"/>
+      <c r="S72" s="86"/>
+      <c r="W72" s="87"/>
+      <c r="X72" s="87"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="R73" s="84"/>
-      <c r="S73" s="84"/>
-      <c r="W73" s="85"/>
-      <c r="X73" s="85"/>
+      <c r="R73" s="86"/>
+      <c r="S73" s="86"/>
+      <c r="W73" s="87"/>
+      <c r="X73" s="87"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="R74" s="84"/>
-      <c r="S74" s="84"/>
-      <c r="W74" s="85"/>
-      <c r="X74" s="85"/>
+      <c r="R74" s="86"/>
+      <c r="S74" s="86"/>
+      <c r="W74" s="87"/>
+      <c r="X74" s="87"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="R75" s="84"/>
-      <c r="S75" s="84"/>
-      <c r="W75" s="85"/>
-      <c r="X75" s="85"/>
+      <c r="R75" s="86"/>
+      <c r="S75" s="86"/>
+      <c r="W75" s="87"/>
+      <c r="X75" s="87"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="R76" s="84"/>
-      <c r="S76" s="84"/>
-      <c r="W76" s="85"/>
-      <c r="X76" s="85"/>
+      <c r="R76" s="86"/>
+      <c r="S76" s="86"/>
+      <c r="W76" s="87"/>
+      <c r="X76" s="87"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="R77" s="84"/>
-      <c r="S77" s="84"/>
-      <c r="W77" s="85"/>
-      <c r="X77" s="85"/>
+      <c r="R77" s="86"/>
+      <c r="S77" s="86"/>
+      <c r="W77" s="87"/>
+      <c r="X77" s="87"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="R78" s="84"/>
-      <c r="S78" s="84"/>
-      <c r="W78" s="85"/>
-      <c r="X78" s="85"/>
+      <c r="R78" s="86"/>
+      <c r="S78" s="86"/>
+      <c r="W78" s="87"/>
+      <c r="X78" s="87"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="R79" s="84"/>
-      <c r="S79" s="84"/>
-      <c r="W79" s="85"/>
-      <c r="X79" s="85"/>
+      <c r="R79" s="86"/>
+      <c r="S79" s="86"/>
+      <c r="W79" s="87"/>
+      <c r="X79" s="87"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="R80" s="84"/>
-      <c r="S80" s="84"/>
-      <c r="W80" s="85"/>
-      <c r="X80" s="85"/>
+      <c r="R80" s="86"/>
+      <c r="S80" s="86"/>
+      <c r="W80" s="87"/>
+      <c r="X80" s="87"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="R81" s="84"/>
-      <c r="S81" s="84"/>
-      <c r="W81" s="85"/>
-      <c r="X81" s="85"/>
+      <c r="R81" s="86"/>
+      <c r="S81" s="86"/>
+      <c r="W81" s="87"/>
+      <c r="X81" s="87"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="R82" s="84"/>
-      <c r="S82" s="84"/>
-      <c r="W82" s="85"/>
-      <c r="X82" s="85"/>
+      <c r="R82" s="86"/>
+      <c r="S82" s="86"/>
+      <c r="W82" s="87"/>
+      <c r="X82" s="87"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="R83" s="84"/>
-      <c r="S83" s="84"/>
-      <c r="W83" s="85"/>
-      <c r="X83" s="85"/>
+      <c r="R83" s="86"/>
+      <c r="S83" s="86"/>
+      <c r="W83" s="87"/>
+      <c r="X83" s="87"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="R84" s="84"/>
-      <c r="S84" s="84"/>
-      <c r="W84" s="85"/>
-      <c r="X84" s="85"/>
+      <c r="R84" s="86"/>
+      <c r="S84" s="86"/>
+      <c r="W84" s="87"/>
+      <c r="X84" s="87"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="R85" s="84"/>
-      <c r="S85" s="84"/>
-      <c r="W85" s="85"/>
-      <c r="X85" s="85"/>
+      <c r="R85" s="86"/>
+      <c r="S85" s="86"/>
+      <c r="W85" s="87"/>
+      <c r="X85" s="87"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="R86" s="84"/>
-      <c r="S86" s="84"/>
-      <c r="W86" s="85"/>
-      <c r="X86" s="85"/>
+      <c r="R86" s="86"/>
+      <c r="S86" s="86"/>
+      <c r="W86" s="87"/>
+      <c r="X86" s="87"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="R87" s="84"/>
-      <c r="S87" s="84"/>
-      <c r="W87" s="85"/>
-      <c r="X87" s="85"/>
+      <c r="R87" s="86"/>
+      <c r="S87" s="86"/>
+      <c r="W87" s="87"/>
+      <c r="X87" s="87"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="R88" s="84"/>
-      <c r="S88" s="84"/>
-      <c r="W88" s="85"/>
-      <c r="X88" s="85"/>
+      <c r="R88" s="86"/>
+      <c r="S88" s="86"/>
+      <c r="W88" s="87"/>
+      <c r="X88" s="87"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="R89" s="84"/>
-      <c r="S89" s="84"/>
-      <c r="W89" s="85"/>
-      <c r="X89" s="85"/>
+      <c r="R89" s="86"/>
+      <c r="S89" s="86"/>
+      <c r="W89" s="87"/>
+      <c r="X89" s="87"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="R90" s="84"/>
-      <c r="S90" s="84"/>
-      <c r="W90" s="85"/>
-      <c r="X90" s="85"/>
+      <c r="R90" s="86"/>
+      <c r="S90" s="86"/>
+      <c r="W90" s="87"/>
+      <c r="X90" s="87"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="R91" s="84"/>
-      <c r="S91" s="84"/>
-      <c r="W91" s="85"/>
-      <c r="X91" s="85"/>
+      <c r="R91" s="86"/>
+      <c r="S91" s="86"/>
+      <c r="W91" s="87"/>
+      <c r="X91" s="87"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="R92" s="84"/>
-      <c r="S92" s="84"/>
-      <c r="W92" s="85"/>
-      <c r="X92" s="85"/>
+      <c r="R92" s="86"/>
+      <c r="S92" s="86"/>
+      <c r="W92" s="87"/>
+      <c r="X92" s="87"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="R93" s="84"/>
-      <c r="S93" s="84"/>
-      <c r="W93" s="85"/>
-      <c r="X93" s="85"/>
+      <c r="R93" s="86"/>
+      <c r="S93" s="86"/>
+      <c r="W93" s="87"/>
+      <c r="X93" s="87"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="R94" s="84"/>
-      <c r="S94" s="84"/>
-      <c r="W94" s="85"/>
-      <c r="X94" s="85"/>
+      <c r="R94" s="86"/>
+      <c r="S94" s="86"/>
+      <c r="W94" s="87"/>
+      <c r="X94" s="87"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="R95" s="84"/>
-      <c r="S95" s="84"/>
-      <c r="W95" s="85"/>
-      <c r="X95" s="85"/>
+      <c r="R95" s="86"/>
+      <c r="S95" s="86"/>
+      <c r="W95" s="87"/>
+      <c r="X95" s="87"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="R96" s="84"/>
-      <c r="S96" s="84"/>
-      <c r="W96" s="85"/>
-      <c r="X96" s="85"/>
+      <c r="R96" s="86"/>
+      <c r="S96" s="86"/>
+      <c r="W96" s="87"/>
+      <c r="X96" s="87"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="R97" s="84"/>
-      <c r="S97" s="84"/>
-      <c r="W97" s="85"/>
-      <c r="X97" s="85"/>
+      <c r="R97" s="86"/>
+      <c r="S97" s="86"/>
+      <c r="W97" s="87"/>
+      <c r="X97" s="87"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="R98" s="84"/>
-      <c r="S98" s="84"/>
-      <c r="W98" s="85"/>
-      <c r="X98" s="85"/>
+      <c r="R98" s="86"/>
+      <c r="S98" s="86"/>
+      <c r="W98" s="87"/>
+      <c r="X98" s="87"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="R99" s="84"/>
-      <c r="S99" s="84"/>
-      <c r="W99" s="85"/>
-      <c r="X99" s="85"/>
+      <c r="R99" s="86"/>
+      <c r="S99" s="86"/>
+      <c r="W99" s="87"/>
+      <c r="X99" s="87"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="R100" s="84"/>
-      <c r="S100" s="84"/>
-      <c r="W100" s="85"/>
-      <c r="X100" s="85"/>
+      <c r="R100" s="86"/>
+      <c r="S100" s="86"/>
+      <c r="W100" s="87"/>
+      <c r="X100" s="87"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="R101" s="84"/>
-      <c r="S101" s="84"/>
-      <c r="W101" s="85"/>
-      <c r="X101" s="85"/>
+      <c r="R101" s="86"/>
+      <c r="S101" s="86"/>
+      <c r="W101" s="87"/>
+      <c r="X101" s="87"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="R102" s="84"/>
-      <c r="S102" s="84"/>
-      <c r="W102" s="85"/>
-      <c r="X102" s="85"/>
+      <c r="R102" s="86"/>
+      <c r="S102" s="86"/>
+      <c r="W102" s="87"/>
+      <c r="X102" s="87"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="R103" s="84"/>
-      <c r="S103" s="84"/>
-      <c r="W103" s="85"/>
-      <c r="X103" s="85"/>
+      <c r="R103" s="86"/>
+      <c r="S103" s="86"/>
+      <c r="W103" s="87"/>
+      <c r="X103" s="87"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="R104" s="84"/>
-      <c r="S104" s="84"/>
-      <c r="W104" s="85"/>
-      <c r="X104" s="85"/>
+      <c r="R104" s="86"/>
+      <c r="S104" s="86"/>
+      <c r="W104" s="87"/>
+      <c r="X104" s="87"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="R105" s="84"/>
-      <c r="S105" s="84"/>
-      <c r="W105" s="85"/>
-      <c r="X105" s="85"/>
+      <c r="R105" s="86"/>
+      <c r="S105" s="86"/>
+      <c r="W105" s="87"/>
+      <c r="X105" s="87"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="R106" s="84"/>
-      <c r="S106" s="84"/>
-      <c r="W106" s="85"/>
-      <c r="X106" s="85"/>
+      <c r="R106" s="86"/>
+      <c r="S106" s="86"/>
+      <c r="W106" s="87"/>
+      <c r="X106" s="87"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="R107" s="84"/>
-      <c r="S107" s="84"/>
-      <c r="W107" s="85"/>
-      <c r="X107" s="85"/>
+      <c r="R107" s="86"/>
+      <c r="S107" s="86"/>
+      <c r="W107" s="87"/>
+      <c r="X107" s="87"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="R108" s="84"/>
-      <c r="S108" s="84"/>
-      <c r="W108" s="85"/>
-      <c r="X108" s="85"/>
+      <c r="R108" s="86"/>
+      <c r="S108" s="86"/>
+      <c r="W108" s="87"/>
+      <c r="X108" s="87"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="R109" s="84"/>
-      <c r="S109" s="84"/>
-      <c r="W109" s="85"/>
-      <c r="X109" s="85"/>
+      <c r="R109" s="86"/>
+      <c r="S109" s="86"/>
+      <c r="W109" s="87"/>
+      <c r="X109" s="87"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="R110" s="84"/>
-      <c r="S110" s="84"/>
-      <c r="W110" s="85"/>
-      <c r="X110" s="85"/>
+      <c r="R110" s="86"/>
+      <c r="S110" s="86"/>
+      <c r="W110" s="87"/>
+      <c r="X110" s="87"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="R111" s="84"/>
-      <c r="S111" s="84"/>
-      <c r="W111" s="85"/>
-      <c r="X111" s="85"/>
+      <c r="R111" s="86"/>
+      <c r="S111" s="86"/>
+      <c r="W111" s="87"/>
+      <c r="X111" s="87"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="R112" s="84"/>
-      <c r="S112" s="84"/>
-      <c r="W112" s="85"/>
-      <c r="X112" s="85"/>
+      <c r="R112" s="86"/>
+      <c r="S112" s="86"/>
+      <c r="W112" s="87"/>
+      <c r="X112" s="87"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="R113" s="84"/>
-      <c r="S113" s="84"/>
-      <c r="W113" s="85"/>
-      <c r="X113" s="85"/>
+      <c r="R113" s="86"/>
+      <c r="S113" s="86"/>
+      <c r="W113" s="87"/>
+      <c r="X113" s="87"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="R114" s="84"/>
-      <c r="S114" s="84"/>
-      <c r="W114" s="85"/>
-      <c r="X114" s="85"/>
+      <c r="R114" s="86"/>
+      <c r="S114" s="86"/>
+      <c r="W114" s="87"/>
+      <c r="X114" s="87"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="R115" s="84"/>
-      <c r="S115" s="84"/>
-      <c r="W115" s="85"/>
-      <c r="X115" s="85"/>
+      <c r="R115" s="86"/>
+      <c r="S115" s="86"/>
+      <c r="W115" s="87"/>
+      <c r="X115" s="87"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="R116" s="84"/>
-      <c r="S116" s="84"/>
-      <c r="W116" s="85"/>
-      <c r="X116" s="85"/>
+      <c r="R116" s="86"/>
+      <c r="S116" s="86"/>
+      <c r="W116" s="87"/>
+      <c r="X116" s="87"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="R117" s="84"/>
-      <c r="S117" s="84"/>
-      <c r="W117" s="85"/>
-      <c r="X117" s="85"/>
+      <c r="R117" s="86"/>
+      <c r="S117" s="86"/>
+      <c r="W117" s="87"/>
+      <c r="X117" s="87"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="R118" s="84"/>
-      <c r="S118" s="84"/>
-      <c r="W118" s="85"/>
-      <c r="X118" s="85"/>
+      <c r="R118" s="86"/>
+      <c r="S118" s="86"/>
+      <c r="W118" s="87"/>
+      <c r="X118" s="87"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="R119" s="84"/>
-      <c r="S119" s="84"/>
-      <c r="W119" s="85"/>
-      <c r="X119" s="85"/>
+      <c r="R119" s="86"/>
+      <c r="S119" s="86"/>
+      <c r="W119" s="87"/>
+      <c r="X119" s="87"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="R120" s="84"/>
-      <c r="S120" s="84"/>
-      <c r="W120" s="85"/>
-      <c r="X120" s="85"/>
+      <c r="R120" s="86"/>
+      <c r="S120" s="86"/>
+      <c r="W120" s="87"/>
+      <c r="X120" s="87"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="R121" s="84"/>
-      <c r="S121" s="84"/>
-      <c r="W121" s="85"/>
-      <c r="X121" s="85"/>
+      <c r="R121" s="86"/>
+      <c r="S121" s="86"/>
+      <c r="W121" s="87"/>
+      <c r="X121" s="87"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="R122" s="84"/>
-      <c r="S122" s="84"/>
-      <c r="W122" s="85"/>
-      <c r="X122" s="85"/>
+      <c r="R122" s="86"/>
+      <c r="S122" s="86"/>
+      <c r="W122" s="87"/>
+      <c r="X122" s="87"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
-      <c r="R123" s="84"/>
-      <c r="S123" s="84"/>
-      <c r="W123" s="85"/>
-      <c r="X123" s="85"/>
+      <c r="R123" s="86"/>
+      <c r="S123" s="86"/>
+      <c r="W123" s="87"/>
+      <c r="X123" s="87"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="R124" s="84"/>
-      <c r="S124" s="84"/>
-      <c r="W124" s="85"/>
-      <c r="X124" s="85"/>
+      <c r="R124" s="86"/>
+      <c r="S124" s="86"/>
+      <c r="W124" s="87"/>
+      <c r="X124" s="87"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="R125" s="84"/>
-      <c r="S125" s="84"/>
-      <c r="W125" s="85"/>
-      <c r="X125" s="85"/>
+      <c r="R125" s="86"/>
+      <c r="S125" s="86"/>
+      <c r="W125" s="87"/>
+      <c r="X125" s="87"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="R126" s="84"/>
-      <c r="S126" s="84"/>
-      <c r="W126" s="85"/>
-      <c r="X126" s="85"/>
+      <c r="R126" s="86"/>
+      <c r="S126" s="86"/>
+      <c r="W126" s="87"/>
+      <c r="X126" s="87"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="R127" s="84"/>
-      <c r="S127" s="84"/>
-      <c r="W127" s="85"/>
-      <c r="X127" s="85"/>
+      <c r="R127" s="86"/>
+      <c r="S127" s="86"/>
+      <c r="W127" s="87"/>
+      <c r="X127" s="87"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="R128" s="84"/>
-      <c r="S128" s="84"/>
-      <c r="W128" s="85"/>
-      <c r="X128" s="85"/>
+      <c r="R128" s="86"/>
+      <c r="S128" s="86"/>
+      <c r="W128" s="87"/>
+      <c r="X128" s="87"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="R129" s="84"/>
-      <c r="S129" s="84"/>
-      <c r="W129" s="85"/>
-      <c r="X129" s="85"/>
+      <c r="R129" s="86"/>
+      <c r="S129" s="86"/>
+      <c r="W129" s="87"/>
+      <c r="X129" s="87"/>
     </row>
     <row r="130" ht="15.75" customHeight="1"/>
     <row r="131" ht="15.75" customHeight="1"/>
@@ -4271,15 +4466,15 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{FB3C7818-4343-4A28-8E26-044A3EA3FFB6}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$BK$9"/>
+    <customSheetView guid="{CD1ADC1F-EDD1-4928-9B54-5CE003589629}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$BK$10"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1006682980"/>
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{D8983E15-4FC1-4A80-93C5-4000FD62EAFE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{15618BF6-7F2C-45DE-8AC8-B0FB1C498E50}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
@@ -4287,7 +4482,7 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{68DFCC14-0523-47BB-B77A-F517A28BB91C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{483C286D-37C2-478D-A8B5-55DAECA2C6C9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
@@ -4295,7 +4490,7 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{65C347E1-C998-4DAB-AADA-CAA2A50B84A3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B7FEAD40-3014-4592-862A-43375AC0CF55}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$BK$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>